<commit_message>
Fixed errors with setup together with Frida
</commit_message>
<xml_diff>
--- a/Minigut.setup_FD.xlsx
+++ b/Minigut.setup_FD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab\Desktop\ph-meter-interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{788ADA4C-2D56-7345-A8A8-07B0308A7C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1989E473-69B8-2145-B1FD-2852A7A8C65E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F86883-2E47-43EE-9FFF-2C64D58D2A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Pump</t>
   </si>
@@ -51,19 +51,22 @@
     <t>Force delay</t>
   </si>
   <si>
-    <t>F.0.1.22_1</t>
-  </si>
-  <si>
-    <t>F.0.1.22_2</t>
-  </si>
-  <si>
-    <t>F.0.1.22_3</t>
-  </si>
-  <si>
-    <t>F.0.1.22_4</t>
-  </si>
-  <si>
     <t>F.0.1.21_1</t>
+  </si>
+  <si>
+    <t>F.0.1.21_2</t>
+  </si>
+  <si>
+    <t>F.0.1.13_1</t>
+  </si>
+  <si>
+    <t>F.0.1.13_2</t>
+  </si>
+  <si>
+    <t>F.0.1.13_3</t>
+  </si>
+  <si>
+    <t>F.0.1.13_4</t>
   </si>
 </sst>
 </file>
@@ -538,19 +541,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="29" width="9.6640625" style="7" customWidth="1"/>
+    <col min="1" max="29" width="9.625" style="7" customWidth="1"/>
     <col min="30" max="32" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -600,7 +603,7 @@
       <c r="AE1"/>
       <c r="AF1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -608,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="11">
         <v>1440</v>
@@ -650,7 +653,7 @@
       <c r="AE2"/>
       <c r="AF2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -658,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="11">
         <v>1440</v>
@@ -700,7 +703,7 @@
       <c r="AE3"/>
       <c r="AF3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -708,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="11">
         <v>1440</v>
@@ -750,7 +753,7 @@
       <c r="AE4"/>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -758,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="11">
         <v>1440</v>
@@ -800,7 +803,7 @@
       <c r="AE5"/>
       <c r="AF5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -808,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D6" s="11">
         <v>1440</v>
@@ -850,7 +853,31 @@
       <c r="AE6"/>
       <c r="AF6"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E7" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F7" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G7" s="13">
+        <v>5</v>
+      </c>
+      <c r="H7" s="13">
+        <v>1</v>
+      </c>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -876,15 +903,31 @@
       <c r="AE7"/>
       <c r="AF7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E8" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F8" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G8" s="13">
+        <v>5</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -910,7 +953,31 @@
       <c r="AE8"/>
       <c r="AF8"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E9" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F9" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G9" s="13">
+        <v>5</v>
+      </c>
+      <c r="H9" s="13">
+        <v>1</v>
+      </c>
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>
@@ -927,7 +994,31 @@
       <c r="AE9"/>
       <c r="AF9"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E10" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F10" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G10" s="13">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
@@ -944,7 +1035,31 @@
       <c r="AE10"/>
       <c r="AF10"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E11" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F11" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G11" s="13">
+        <v>5</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1</v>
+      </c>
       <c r="R11"/>
       <c r="S11"/>
       <c r="T11"/>
@@ -961,7 +1076,31 @@
       <c r="AE11"/>
       <c r="AF11"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E12" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F12" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G12" s="13">
+        <v>5</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1</v>
+      </c>
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12"/>
@@ -978,6 +1117,32 @@
       <c r="AE12"/>
       <c r="AF12"/>
     </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1440</v>
+      </c>
+      <c r="E13" s="12">
+        <v>5.6</v>
+      </c>
+      <c r="F13" s="12">
+        <v>6.8</v>
+      </c>
+      <c r="G13" s="13">
+        <v>5</v>
+      </c>
+      <c r="H13" s="13">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed bugs doing actual test run
</commit_message>
<xml_diff>
--- a/Minigut.setup_FD.xlsx
+++ b/Minigut.setup_FD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab\Desktop\ph-meter-interface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F86883-2E47-43EE-9FFF-2C64D58D2A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07601DA0-20B2-4052-B292-D596549A248D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Pump</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>F.0.1.13_4</t>
+  </si>
+  <si>
+    <t>F.0.1.21_3</t>
+  </si>
+  <si>
+    <t>F.0.1.21_4</t>
+  </si>
+  <si>
+    <t>F.0.1.22_1</t>
+  </si>
+  <si>
+    <t>F.0.1.22_2</t>
+  </si>
+  <si>
+    <t>F.0.1.22_3</t>
+  </si>
+  <si>
+    <t>F.0.1.22_4</t>
   </si>
 </sst>
 </file>
@@ -544,7 +562,7 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -626,7 +644,7 @@
         <v>5</v>
       </c>
       <c r="H2" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2"/>
       <c r="J2"/>
@@ -676,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="H3" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3"/>
       <c r="J3"/>
@@ -726,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -776,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I5"/>
       <c r="J5"/>
@@ -826,7 +844,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6"/>
       <c r="J6"/>
@@ -876,7 +894,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -911,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D8" s="11">
         <v>1440</v>
@@ -926,7 +944,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
@@ -961,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D9" s="11">
         <v>1440</v>
@@ -976,7 +994,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9"/>
       <c r="S9"/>
@@ -1002,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D10" s="11">
         <v>1440</v>
@@ -1017,7 +1035,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10"/>
       <c r="S10"/>
@@ -1043,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D11" s="11">
         <v>1440</v>
@@ -1058,7 +1076,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11"/>
       <c r="S11"/>
@@ -1084,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D12" s="11">
         <v>1440</v>
@@ -1099,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12"/>
       <c r="S12"/>
@@ -1125,7 +1143,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D13" s="11">
         <v>1440</v>
@@ -1140,7 +1158,7 @@
         <v>5</v>
       </c>
       <c r="H13" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for multiple pumps, depending on the pH value.
</commit_message>
<xml_diff>
--- a/Minigut.setup_FD.xlsx
+++ b/Minigut.setup_FD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab\Desktop\ph-meter-interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jespersamsobirch/OneDrive - SniprBiome/ph-meter-interface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07601DA0-20B2-4052-B292-D596549A248D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A0BF40-DAC4-D342-B040-4C44AD876D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Pump</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>F.0.1.22_4</t>
+  </si>
+  <si>
+    <t>Dose multiplier interval</t>
   </si>
 </sst>
 </file>
@@ -562,16 +565,18 @@
   <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="29" width="9.625" style="7" customWidth="1"/>
+    <col min="1" max="7" width="9.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="16" style="7" customWidth="1"/>
+    <col min="9" max="29" width="9.6640625" style="7" customWidth="1"/>
     <col min="30" max="32" width="11" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -594,9 +599,11 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1"/>
       <c r="J1"/>
       <c r="K1"/>
       <c r="L1"/>
@@ -621,7 +628,7 @@
       <c r="AE1"/>
       <c r="AF1"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -644,9 +651,11 @@
         <v>5</v>
       </c>
       <c r="H2" s="13">
-        <v>2</v>
-      </c>
-      <c r="I2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="13">
+        <v>2</v>
+      </c>
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -671,7 +680,7 @@
       <c r="AE2"/>
       <c r="AF2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -694,9 +703,11 @@
         <v>5</v>
       </c>
       <c r="H3" s="13">
-        <v>2</v>
-      </c>
-      <c r="I3"/>
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="13">
+        <v>2</v>
+      </c>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
@@ -721,7 +732,7 @@
       <c r="AE3"/>
       <c r="AF3"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>3</v>
       </c>
@@ -744,9 +755,11 @@
         <v>5</v>
       </c>
       <c r="H4" s="13">
-        <v>2</v>
-      </c>
-      <c r="I4"/>
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="13">
+        <v>2</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -771,7 +784,7 @@
       <c r="AE4"/>
       <c r="AF4"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="8">
         <v>4</v>
       </c>
@@ -794,9 +807,11 @@
         <v>5</v>
       </c>
       <c r="H5" s="13">
-        <v>2</v>
-      </c>
-      <c r="I5"/>
+        <v>0.1</v>
+      </c>
+      <c r="I5" s="13">
+        <v>2</v>
+      </c>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
@@ -821,7 +836,7 @@
       <c r="AE5"/>
       <c r="AF5"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="8">
         <v>5</v>
       </c>
@@ -844,9 +859,11 @@
         <v>5</v>
       </c>
       <c r="H6" s="13">
-        <v>2</v>
-      </c>
-      <c r="I6"/>
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="13">
+        <v>2</v>
+      </c>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -871,7 +888,7 @@
       <c r="AE6"/>
       <c r="AF6"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="8">
         <v>6</v>
       </c>
@@ -894,9 +911,11 @@
         <v>5</v>
       </c>
       <c r="H7" s="13">
-        <v>2</v>
-      </c>
-      <c r="I7"/>
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="13">
+        <v>2</v>
+      </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -921,7 +940,7 @@
       <c r="AE7"/>
       <c r="AF7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="8">
         <v>7</v>
       </c>
@@ -944,9 +963,11 @@
         <v>5</v>
       </c>
       <c r="H8" s="13">
-        <v>2</v>
-      </c>
-      <c r="I8"/>
+        <v>0.1</v>
+      </c>
+      <c r="I8" s="13">
+        <v>2</v>
+      </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
@@ -971,7 +992,7 @@
       <c r="AE8"/>
       <c r="AF8"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="8">
         <v>8</v>
       </c>
@@ -994,6 +1015,9 @@
         <v>5</v>
       </c>
       <c r="H9" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I9" s="13">
         <v>2</v>
       </c>
       <c r="R9"/>
@@ -1012,7 +1036,7 @@
       <c r="AE9"/>
       <c r="AF9"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="8">
         <v>9</v>
       </c>
@@ -1035,6 +1059,9 @@
         <v>5</v>
       </c>
       <c r="H10" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I10" s="13">
         <v>2</v>
       </c>
       <c r="R10"/>
@@ -1053,7 +1080,7 @@
       <c r="AE10"/>
       <c r="AF10"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>10</v>
       </c>
@@ -1076,6 +1103,9 @@
         <v>5</v>
       </c>
       <c r="H11" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I11" s="13">
         <v>2</v>
       </c>
       <c r="R11"/>
@@ -1094,7 +1124,7 @@
       <c r="AE11"/>
       <c r="AF11"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>11</v>
       </c>
@@ -1117,6 +1147,9 @@
         <v>5</v>
       </c>
       <c r="H12" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I12" s="13">
         <v>2</v>
       </c>
       <c r="R12"/>
@@ -1135,7 +1168,7 @@
       <c r="AE12"/>
       <c r="AF12"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>12</v>
       </c>
@@ -1158,6 +1191,9 @@
         <v>5</v>
       </c>
       <c r="H13" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="13">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed dependency of dose multiplier and updated documentation.
</commit_message>
<xml_diff>
--- a/Minigut.setup_FD.xlsx
+++ b/Minigut.setup_FD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lab\Desktop\ph-meter-interface\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://snipr-my.sharepoint.com/personal/jsb_sniprbiome_com/Documents/ph-meter-interface/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06404B5B-D082-42CF-892E-69ADD0FD30ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{06404B5B-D082-42CF-892E-69ADD0FD30ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06510684-BB1F-8640-BA9B-04822830692D}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="1170" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5620" yWindow="1180" windowWidth="21600" windowHeight="11380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Pump</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>F.0.1.22_4</t>
-  </si>
-  <si>
-    <t>Dose multiplier interval</t>
   </si>
 </sst>
 </file>
@@ -561,20 +558,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="9.625" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="29" width="9.625" customWidth="1"/>
+    <col min="1" max="28" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -597,13 +592,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -626,13 +618,10 @@
         <v>5</v>
       </c>
       <c r="H2" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -655,13 +644,10 @@
         <v>5</v>
       </c>
       <c r="H3" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I3" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -684,13 +670,10 @@
         <v>5</v>
       </c>
       <c r="H4" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I4" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -713,13 +696,10 @@
         <v>5</v>
       </c>
       <c r="H5" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I5" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -742,13 +722,10 @@
         <v>5</v>
       </c>
       <c r="H6" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I6" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -771,13 +748,10 @@
         <v>5</v>
       </c>
       <c r="H7" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I7" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -800,13 +774,10 @@
         <v>5</v>
       </c>
       <c r="H8" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I8" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -829,13 +800,10 @@
         <v>5</v>
       </c>
       <c r="H9" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I9" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -858,13 +826,10 @@
         <v>5</v>
       </c>
       <c r="H10" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I10" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -887,13 +852,10 @@
         <v>5</v>
       </c>
       <c r="H11" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -916,13 +878,10 @@
         <v>5</v>
       </c>
       <c r="H12" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I12" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -945,9 +904,6 @@
         <v>5</v>
       </c>
       <c r="H13" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="I13" s="12">
         <v>2</v>
       </c>
     </row>

</xml_diff>